<commit_message>
:sparkles: New tables for Monomorphic species
</commit_message>
<xml_diff>
--- a/tables/BC_Ring_Table.xlsx
+++ b/tables/BC_Ring_Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael\R_projects\ithomiini_convergence\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CFA7A6-DAD8-4406-A85F-556DD772DC0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C926B-D4A7-4155-AC32-51F3F67CB9B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Print_Area" localSheetId="0">Feuil2!$B$2:$J$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil2!$B$2:$J$46</definedName>
+    <definedName name="Print_Area" localSheetId="0">Feuil2!$B$2:$I$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil2!$B$2:$I$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="154">
   <si>
     <t>EURIMEDIA</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Mimicry ring</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>N OMUs</t>
   </si>
   <si>
@@ -179,24 +176,6 @@
   </si>
   <si>
     <t>p-value</t>
-  </si>
-  <si>
-    <t>Andean</t>
-  </si>
-  <si>
-    <t>Amazonian</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>Central Am.</t>
-  </si>
-  <si>
-    <t>Mata Atl.</t>
-  </si>
-  <si>
-    <t>Mata. Atl.</t>
   </si>
   <si>
     <t>NA</t>
@@ -893,24 +872,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:J46"/>
+  <dimension ref="B2:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J46"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="10" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="9" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
@@ -935,1288 +913,1153 @@
       <c r="I2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>50</v>
+      <c r="C3" s="1">
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
         <v>0</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5">
+        <v>85</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3570</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="5">
-        <v>85</v>
-      </c>
-      <c r="E4" s="5">
-        <v>3570</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>50</v>
+      <c r="C5" s="1">
+        <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
         <v>36</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>51</v>
+      <c r="C6" s="5">
+        <v>12</v>
       </c>
       <c r="D6" s="5">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5">
         <v>66</v>
       </c>
+      <c r="E6" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F6" s="5" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
+        <v>151</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45</v>
       </c>
       <c r="D7" s="1">
-        <v>45</v>
-      </c>
-      <c r="E7" s="1">
         <v>990</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>52</v>
+      <c r="C8" s="5">
+        <v>20</v>
       </c>
       <c r="D8" s="5">
-        <v>20</v>
-      </c>
-      <c r="E8" s="5">
         <v>190</v>
       </c>
+      <c r="E8" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="5" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>94</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>50</v>
+      <c r="C9" s="1">
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
         <v>0</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>50</v>
+      <c r="C10" s="5">
+        <v>40</v>
       </c>
       <c r="D10" s="5">
-        <v>40</v>
-      </c>
-      <c r="E10" s="5">
         <v>780</v>
       </c>
+      <c r="E10" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="F10" s="5" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
-        <v>51</v>
+      <c r="C11" s="1">
+        <v>15</v>
       </c>
       <c r="D11" s="1">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1">
         <v>105</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>51</v>
+      <c r="C12" s="5">
+        <v>4</v>
       </c>
       <c r="D12" s="5">
-        <v>4</v>
-      </c>
-      <c r="E12" s="5">
         <v>6</v>
       </c>
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F12" s="5" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="5">
+        <v>72</v>
+      </c>
+      <c r="H12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
-        <v>50</v>
+      <c r="C13" s="1">
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
-      <c r="E13" s="1">
-        <v>3</v>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="1">
+        <v>95</v>
+      </c>
+      <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>51</v>
+      <c r="C14" s="5">
+        <v>11</v>
       </c>
       <c r="D14" s="5">
-        <v>11</v>
-      </c>
-      <c r="E14" s="5">
         <v>55</v>
       </c>
+      <c r="E14" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F14" s="5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="C15" t="s">
-        <v>52</v>
+      <c r="C15" s="1">
+        <v>35</v>
       </c>
       <c r="D15" s="1">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1">
         <v>595</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>53</v>
+      <c r="C16" s="5">
+        <v>18</v>
       </c>
       <c r="D16" s="5">
-        <v>18</v>
-      </c>
-      <c r="E16" s="5">
         <v>153</v>
       </c>
+      <c r="E16" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="F16" s="5" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>54</v>
+      <c r="C17" s="1">
+        <v>7</v>
       </c>
       <c r="D17" s="1">
-        <v>7</v>
-      </c>
-      <c r="E17" s="1">
         <v>21</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>52</v>
+      <c r="C18" s="5">
+        <v>53</v>
       </c>
       <c r="D18" s="5">
-        <v>53</v>
-      </c>
-      <c r="E18" s="5">
         <v>1378</v>
       </c>
+      <c r="E18" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="F18" s="5" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C19" t="s">
-        <v>50</v>
+      <c r="C19" s="1">
+        <v>30</v>
       </c>
       <c r="D19" s="1">
-        <v>30</v>
-      </c>
-      <c r="E19" s="1">
         <v>435</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>50</v>
+      <c r="C20" s="5">
+        <v>1</v>
       </c>
       <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="E20" s="5">
         <v>0</v>
       </c>
+      <c r="E20" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="F20" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" t="s">
-        <v>51</v>
+      <c r="C21" s="1">
+        <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>6</v>
-      </c>
-      <c r="E21" s="1">
         <v>15</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="1">
+        <v>99</v>
+      </c>
+      <c r="H21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>52</v>
+      <c r="C22" s="5">
+        <v>66</v>
       </c>
       <c r="D22" s="5">
-        <v>66</v>
-      </c>
-      <c r="E22" s="5">
         <v>2145</v>
       </c>
+      <c r="E22" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="F22" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
-        <v>50</v>
+      <c r="C23" s="1">
+        <v>21</v>
       </c>
       <c r="D23" s="1">
-        <v>21</v>
-      </c>
-      <c r="E23" s="1">
         <v>210</v>
       </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F23" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>55</v>
+      <c r="C24" s="5">
+        <v>5</v>
       </c>
       <c r="D24" s="5">
-        <v>5</v>
-      </c>
-      <c r="E24" s="5">
         <v>10</v>
       </c>
+      <c r="E24" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F24" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I24" s="5">
+        <v>102</v>
+      </c>
+      <c r="H24" s="5">
         <v>1</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>15</v>
       </c>
-      <c r="C25" t="s">
-        <v>51</v>
+      <c r="C25" s="1">
+        <v>16</v>
       </c>
       <c r="D25" s="1">
-        <v>16</v>
-      </c>
-      <c r="E25" s="1">
         <v>120</v>
       </c>
+      <c r="E25" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="F25" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>52</v>
+      <c r="C26" s="5">
+        <v>64</v>
       </c>
       <c r="D26" s="5">
-        <v>64</v>
-      </c>
-      <c r="E26" s="5">
         <v>2016</v>
       </c>
+      <c r="E26" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="F26" s="5" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>20</v>
       </c>
-      <c r="C27" t="s">
-        <v>50</v>
+      <c r="C27" s="1">
+        <v>5</v>
       </c>
       <c r="D27" s="1">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1">
         <v>10</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F27" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" s="1">
+        <v>99</v>
+      </c>
+      <c r="H27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>50</v>
+      <c r="C28" s="5">
+        <v>14</v>
       </c>
       <c r="D28" s="5">
-        <v>14</v>
-      </c>
-      <c r="E28" s="5">
         <v>91</v>
       </c>
+      <c r="E28" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="F28" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
-        <v>50</v>
+      <c r="C29" s="1">
+        <v>14</v>
       </c>
       <c r="D29" s="1">
-        <v>14</v>
-      </c>
-      <c r="E29" s="1">
         <v>91</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="F29" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>50</v>
+      <c r="C30" s="5">
+        <v>13</v>
       </c>
       <c r="D30" s="5">
-        <v>13</v>
-      </c>
-      <c r="E30" s="5">
         <v>78</v>
       </c>
+      <c r="E30" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="F30" s="5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" t="s">
-        <v>51</v>
+      <c r="C31" s="1">
+        <v>16</v>
       </c>
       <c r="D31" s="1">
-        <v>16</v>
-      </c>
-      <c r="E31" s="1">
         <v>120</v>
       </c>
+      <c r="E31" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F31" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>50</v>
+      <c r="C32" s="5">
+        <v>19</v>
       </c>
       <c r="D32" s="5">
-        <v>19</v>
-      </c>
-      <c r="E32" s="5">
         <v>171</v>
       </c>
+      <c r="E32" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="F32" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" t="s">
-        <v>50</v>
+      <c r="C33" s="1">
+        <v>39</v>
       </c>
       <c r="D33" s="1">
-        <v>39</v>
-      </c>
-      <c r="E33" s="1">
         <v>741</v>
       </c>
+      <c r="E33" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F33" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>53</v>
+      <c r="C34" s="5">
+        <v>7</v>
       </c>
       <c r="D34" s="5">
-        <v>7</v>
-      </c>
-      <c r="E34" s="5">
         <v>21</v>
       </c>
+      <c r="E34" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="F34" s="5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>24</v>
       </c>
-      <c r="C35" t="s">
-        <v>50</v>
+      <c r="C35" s="1">
+        <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="1">
         <v>1</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I35" s="1">
+      <c r="I35" s="8">
         <v>1</v>
       </c>
-      <c r="J35" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>52</v>
+      <c r="C36" s="5">
+        <v>10</v>
       </c>
       <c r="D36" s="5">
-        <v>10</v>
-      </c>
-      <c r="E36" s="5">
         <v>45</v>
       </c>
+      <c r="E36" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="F36" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
-        <v>50</v>
+      <c r="C37" s="1">
+        <v>1</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1">
         <v>0</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F37" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>50</v>
+      <c r="C38" s="5">
+        <v>9</v>
       </c>
       <c r="D38" s="5">
-        <v>9</v>
-      </c>
-      <c r="E38" s="5">
         <v>36</v>
       </c>
+      <c r="E38" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="F38" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="C39" t="s">
-        <v>50</v>
+      <c r="C39" s="1">
+        <v>6</v>
       </c>
       <c r="D39" s="1">
-        <v>6</v>
-      </c>
-      <c r="E39" s="1">
         <v>15</v>
       </c>
+      <c r="E39" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="F39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I39" s="1">
+        <v>54</v>
+      </c>
+      <c r="H39" s="1">
         <v>1</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>51</v>
+      <c r="C40" s="5">
+        <v>9</v>
       </c>
       <c r="D40" s="5">
-        <v>9</v>
-      </c>
-      <c r="E40" s="5">
         <v>36</v>
       </c>
+      <c r="E40" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="F40" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>36</v>
       </c>
-      <c r="C41" t="s">
-        <v>50</v>
+      <c r="C41" s="1">
+        <v>20</v>
       </c>
       <c r="D41" s="1">
-        <v>20</v>
-      </c>
-      <c r="E41" s="1">
         <v>190</v>
       </c>
+      <c r="E41" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="F41" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>50</v>
+        <v>153</v>
+      </c>
+      <c r="C42" s="5">
+        <v>11</v>
       </c>
       <c r="D42" s="5">
-        <v>11</v>
-      </c>
-      <c r="E42" s="5">
         <v>55</v>
       </c>
+      <c r="E42" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="F42" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>34</v>
       </c>
-      <c r="C43" t="s">
-        <v>50</v>
+      <c r="C43" s="1">
+        <v>8</v>
       </c>
       <c r="D43" s="1">
-        <v>8</v>
-      </c>
-      <c r="E43" s="1">
         <v>28</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>90</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>50</v>
+        <v>152</v>
+      </c>
+      <c r="C44" s="5">
+        <v>8</v>
       </c>
       <c r="D44" s="5">
-        <v>8</v>
-      </c>
-      <c r="E44" s="5">
         <v>28</v>
       </c>
+      <c r="E44" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="F44" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>28</v>
       </c>
-      <c r="C45" t="s">
-        <v>50</v>
+      <c r="C45" s="1">
+        <v>3</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
-      <c r="E45" s="1">
-        <v>3</v>
+      <c r="E45" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" s="1">
+        <v>111</v>
+      </c>
+      <c r="H45" s="1">
         <v>1</v>
       </c>
-      <c r="J45" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I45" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>51</v>
+      <c r="C46" s="10">
+        <v>1</v>
       </c>
       <c r="D46" s="10">
-        <v>1</v>
-      </c>
-      <c r="E46" s="10">
         <v>0</v>
       </c>
+      <c r="E46" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="F46" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J46" s="11" t="s">
-        <v>56</v>
+        <v>49</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B1:J46">
+  <sortState ref="B1:I46">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>